<commit_message>
corrections to tower height
</commit_message>
<xml_diff>
--- a/Documentation/tower_data.xlsx
+++ b/Documentation/tower_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egaertne\WISDEM2\wisdem\NREL15mw_ORWT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615BD14D-6163-4A48-AD6F-54AA762BB8CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E525CB7B-A26B-44F7-9CE6-1657B1F95C1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BFE80E2-434A-464C-9DED-2A26FA0A145D}"/>
+    <workbookView xWindow="-28440" yWindow="345" windowWidth="19185" windowHeight="10200" xr2:uid="{7BFE80E2-434A-464C-9DED-2A26FA0A145D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tower_Geometry" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
   <dimension ref="A2:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +683,7 @@
         <v>3.6754719999999998E-2</v>
       </c>
       <c r="D14">
-        <v>146.18</v>
+        <v>145</v>
       </c>
       <c r="E14">
         <v>6.7175479999999999</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>146.18</v>
+        <v>145</v>
       </c>
       <c r="B23" s="5">
         <v>3.062863E-2</v>

</xml_diff>

<commit_message>
Correcting to tower properties, RNA masses and interias + preliminary documentation, added stiffness/damping for yaw and drivetrain
</commit_message>
<xml_diff>
--- a/Documentation/tower_data.xlsx
+++ b/Documentation/tower_data.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egaertne\WISDEM2\wisdem\NREL15mw_ORWT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E525CB7B-A26B-44F7-9CE6-1657B1F95C1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93CE2F1-D5BE-4C92-A95D-204F6C51CC73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28440" yWindow="345" windowWidth="19185" windowHeight="10200" xr2:uid="{7BFE80E2-434A-464C-9DED-2A26FA0A145D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7BFE80E2-434A-464C-9DED-2A26FA0A145D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tower_Geometry" sheetId="1" r:id="rId1"/>
-    <sheet name="Tower_Elastic_Properties" sheetId="2" r:id="rId2"/>
+    <sheet name="Tower_Elastic_Properties" sheetId="4" r:id="rId2"/>
     <sheet name="Materials" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Tower_Elastic_Properties!$A$4:$A$23</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Tower_Elastic_Properties!$D$4:$D$23</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -119,7 +123,7 @@
     <t>kg/m**3</t>
   </si>
   <si>
-    <t>BModes Sectional Properties</t>
+    <t>Input Sectional Properties for Bmodes</t>
   </si>
 </sst>
 </file>
@@ -486,18 +490,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED6BB49-C631-4A05-A4BA-B5BF79F8585F}">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1"/>
+    <col min="1" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="3.26953125" customWidth="1"/>
+    <col min="4" max="5" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -512,7 +516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -527,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -542,7 +546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>15</v>
       </c>
@@ -557,7 +561,7 @@
         <v>9.9999939999999992</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>15</v>
       </c>
@@ -572,7 +576,7 @@
         <v>9.8932979999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>30</v>
       </c>
@@ -587,7 +591,7 @@
         <v>9.5012270000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>30</v>
       </c>
@@ -602,7 +606,7 @@
         <v>9.0738160000000008</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>45</v>
       </c>
@@ -617,7 +621,7 @@
         <v>8.7337340000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>45</v>
       </c>
@@ -632,7 +636,7 @@
         <v>8.4812589999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>60</v>
       </c>
@@ -647,7 +651,7 @@
         <v>8.2546970000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>60</v>
       </c>
@@ -661,7 +665,7 @@
         <v>8.0872309999999992</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>75</v>
       </c>
@@ -675,7 +679,7 @@
         <v>7.5125270000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>75</v>
       </c>
@@ -689,7 +693,7 @@
         <v>6.7175479999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>90</v>
       </c>
@@ -697,7 +701,7 @@
         <v>3.6754719999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>90</v>
       </c>
@@ -705,7 +709,7 @@
         <v>3.345327E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>105</v>
       </c>
@@ -713,7 +717,7 @@
         <v>3.345327E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>105</v>
       </c>
@@ -721,7 +725,7 @@
         <v>2.984231E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>120</v>
       </c>
@@ -729,7 +733,7 @@
         <v>2.984231E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>120</v>
       </c>
@@ -737,7 +741,7 @@
         <v>2.6228640000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>135</v>
       </c>
@@ -745,7 +749,7 @@
         <v>2.6228640000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>135</v>
       </c>
@@ -753,7 +757,7 @@
         <v>3.062863E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>145</v>
       </c>
@@ -767,21 +771,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEEFA01E-65DA-412C-BA17-FBCB2E8B91F5}">
-  <dimension ref="A1:M14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A7482D-9351-4154-8734-5DF3698F8469}">
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -822,7 +826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -863,7 +867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -904,9 +908,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>0.1</v>
+        <v>0.10344827586209999</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -915,25 +919,25 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>11516.348691220001</v>
+        <v>12080.321450040001</v>
       </c>
       <c r="E5" s="1">
-        <v>142609.89181299999</v>
+        <v>149524.46469540001</v>
       </c>
       <c r="F5" s="1">
-        <v>142609.89181299999</v>
+        <v>149524.46469540001</v>
       </c>
       <c r="G5" s="1">
-        <v>3633373039822</v>
+        <v>3809540501792</v>
       </c>
       <c r="H5" s="1">
-        <v>3633373039822</v>
+        <v>3809540501792</v>
       </c>
       <c r="I5" s="1">
-        <v>2881264820579</v>
+        <v>3020965617921</v>
       </c>
       <c r="J5" s="1">
-        <v>293410157738.09998</v>
+        <v>307778890446.90002</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -945,9 +949,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>0.2</v>
+        <v>0.10345517241380001</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -956,25 +960,25 @@
         <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>10383.53417728</v>
+        <v>11246.843648689999</v>
       </c>
       <c r="E6" s="1">
-        <v>120845.4871266</v>
+        <v>139302.90007800001</v>
       </c>
       <c r="F6" s="1">
-        <v>120845.4871266</v>
+        <v>139302.90007800001</v>
       </c>
       <c r="G6" s="1">
-        <v>3078865914054</v>
+        <v>3549118473325</v>
       </c>
       <c r="H6" s="1">
-        <v>3078865914054</v>
+        <v>3549118473325</v>
       </c>
       <c r="I6" s="1">
-        <v>2441540669845</v>
+        <v>2814450949346</v>
       </c>
       <c r="J6" s="1">
-        <v>264548641459.39999</v>
+        <v>286543787227.70001</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
@@ -986,9 +990,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>0.3</v>
+        <v>0.20689655172409999</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -997,25 +1001,25 @@
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>9537.4493778579999</v>
+        <v>11126.299898560001</v>
       </c>
       <c r="E7" s="1">
-        <v>102466.44812450001</v>
+        <v>134871.64993129999</v>
       </c>
       <c r="F7" s="1">
-        <v>102466.44812450001</v>
+        <v>134871.64993129999</v>
       </c>
       <c r="G7" s="1">
-        <v>2610610143298</v>
+        <v>3436220380415</v>
       </c>
       <c r="H7" s="1">
-        <v>2610610143298</v>
+        <v>3436220380415</v>
       </c>
       <c r="I7" s="1">
-        <v>2070213843635</v>
+        <v>2724922761669</v>
       </c>
       <c r="J7" s="1">
-        <v>242992340837.20001</v>
+        <v>283472608880.40002</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
@@ -1027,9 +1031,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>0.4</v>
+        <v>0.20690344827589999</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -1038,25 +1042,25 @@
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>8687.1328513629996</v>
+        <v>10448.901297980001</v>
       </c>
       <c r="E8" s="1">
-        <v>85472.543118400004</v>
+        <v>126731.3834704</v>
       </c>
       <c r="F8" s="1">
-        <v>85472.543118400004</v>
+        <v>126731.3834704</v>
       </c>
       <c r="G8" s="1">
-        <v>2177644410660</v>
+        <v>3228825056572</v>
       </c>
       <c r="H8" s="1">
-        <v>2177644410660</v>
+        <v>3228825056572</v>
       </c>
       <c r="I8" s="1">
-        <v>1726872017653</v>
+        <v>2560458269861</v>
       </c>
       <c r="J8" s="1">
-        <v>221328225512.39999</v>
+        <v>266214045808.5</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
@@ -1068,9 +1072,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>0.5</v>
+        <v>0.31034482758620002</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -1079,25 +1083,25 @@
         <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>7829.4708272110001</v>
+        <v>10033.03017439</v>
       </c>
       <c r="E9" s="1">
-        <v>70628.023619839994</v>
+        <v>112193.9275275</v>
       </c>
       <c r="F9" s="1">
-        <v>70628.023619839994</v>
+        <v>112193.9275275</v>
       </c>
       <c r="G9" s="1">
-        <v>1799440092225</v>
+        <v>2858444013440</v>
       </c>
       <c r="H9" s="1">
-        <v>1799440092225</v>
+        <v>2858444013440</v>
       </c>
       <c r="I9" s="1">
-        <v>1426955993135</v>
+        <v>2266746102658</v>
       </c>
       <c r="J9" s="1">
-        <v>199476963750.60001</v>
+        <v>255618603169.20001</v>
       </c>
       <c r="K9" s="1">
         <v>0</v>
@@ -1109,9 +1113,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>0.6</v>
+        <v>0.31035172413790002</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1120,25 +1124,25 @@
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>6902.4037257509999</v>
+        <v>9633.7537031859993</v>
       </c>
       <c r="E10" s="1">
-        <v>55877.387547589999</v>
+        <v>107767.376841</v>
       </c>
       <c r="F10" s="1">
-        <v>55877.387547589999</v>
+        <v>107767.376841</v>
       </c>
       <c r="G10" s="1">
-        <v>1423627708219</v>
+        <v>2745665652001</v>
       </c>
       <c r="H10" s="1">
-        <v>1423627708219</v>
+        <v>2745665652001</v>
       </c>
       <c r="I10" s="1">
-        <v>1128936772618</v>
+        <v>2177312862037</v>
       </c>
       <c r="J10" s="1">
-        <v>175857419764.39999</v>
+        <v>245445954221.29999</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -1150,9 +1154,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>0.7</v>
+        <v>0.4137931034483</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -1161,25 +1165,25 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>5969.3332106429998</v>
+        <v>9198.5169740649999</v>
       </c>
       <c r="E11" s="1">
-        <v>42982.171867700003</v>
+        <v>93811.253487880007</v>
       </c>
       <c r="F11" s="1">
-        <v>42982.171867700003</v>
+        <v>93811.253487880007</v>
       </c>
       <c r="G11" s="1">
-        <v>1095087181343</v>
+        <v>2390095630264</v>
       </c>
       <c r="H11" s="1">
-        <v>1095087181343</v>
+        <v>2390095630264</v>
       </c>
       <c r="I11" s="1">
-        <v>868404134804.69995</v>
+        <v>1895345834800</v>
       </c>
       <c r="J11" s="1">
-        <v>152084922564.20001</v>
+        <v>234357120358.29999</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
@@ -1191,9 +1195,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>0.8</v>
+        <v>0.4138</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -1202,25 +1206,25 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>5097.579026372</v>
+        <v>8777.5400660449995</v>
       </c>
       <c r="E12" s="1">
-        <v>33564.047324960004</v>
+        <v>89554.919507650004</v>
       </c>
       <c r="F12" s="1">
-        <v>33564.047324960004</v>
+        <v>89554.919507650004</v>
       </c>
       <c r="G12" s="1">
-        <v>855134963693.30005</v>
+        <v>2281654000195</v>
       </c>
       <c r="H12" s="1">
-        <v>855134963693.30005</v>
+        <v>2281654000195</v>
       </c>
       <c r="I12" s="1">
-        <v>678122026208.80005</v>
+        <v>1809351622155</v>
       </c>
       <c r="J12" s="1">
-        <v>129874624875.7</v>
+        <v>223631594039.39999</v>
       </c>
       <c r="K12" s="1">
         <v>0</v>
@@ -1232,9 +1236,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>0.9</v>
+        <v>0.51724137931030001</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -1243,25 +1247,25 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>4628.8370819290003</v>
+        <v>8447.1489700670008</v>
       </c>
       <c r="E13" s="1">
-        <v>25967.17951966</v>
+        <v>79818.23217494</v>
       </c>
       <c r="F13" s="1">
-        <v>25967.17951966</v>
+        <v>79818.23217494</v>
       </c>
       <c r="G13" s="1">
-        <v>661584191583.59998</v>
+        <v>2033585533119</v>
       </c>
       <c r="H13" s="1">
-        <v>661584191583.59998</v>
+        <v>2033585533119</v>
       </c>
       <c r="I13" s="1">
-        <v>524636263925.79999</v>
+        <v>1612633327764</v>
       </c>
       <c r="J13" s="1">
-        <v>117932154953.60001</v>
+        <v>215213986498.5</v>
       </c>
       <c r="K13" s="1">
         <v>0</v>
@@ -1273,44 +1277,413 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
+        <v>0.51724827586209998</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>7883.1582149400001</v>
+      </c>
+      <c r="E14" s="1">
+        <v>74533.789468849995</v>
+      </c>
+      <c r="F14" s="1">
+        <v>74533.789468849995</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1898950050162</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1898950050162</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1505867389778</v>
+      </c>
+      <c r="J14" s="1">
+        <v>200844795285.10001</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>0.62068965517240005</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>7654.3234125070003</v>
+      </c>
+      <c r="E15" s="1">
+        <v>68229.685404210002</v>
+      </c>
+      <c r="F15" s="1">
+        <v>68229.685404210002</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1738335933865</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1738335933865</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1378500395555</v>
+      </c>
+      <c r="J15" s="1">
+        <v>195014609235.89999</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>0.62069655172409999</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6969.4939707189997</v>
+      </c>
+      <c r="E16" s="1">
+        <v>62173.362132590002</v>
+      </c>
+      <c r="F16" s="1">
+        <v>62173.362132590002</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1584034704015</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1584034704015</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1256139520284</v>
+      </c>
+      <c r="J16" s="1">
+        <v>177566725368.60001</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>0.72413793103449997</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6782.5909927980001</v>
+      </c>
+      <c r="E17" s="1">
+        <v>57304.388171869999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>57304.388171869999</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1459984412022</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1459984412022</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1157767638734</v>
+      </c>
+      <c r="J17" s="1">
+        <v>172804866058.5</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>0.72414482758620002</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6053.1245671030001</v>
+      </c>
+      <c r="E18" s="1">
+        <v>51185.933780129999</v>
+      </c>
+      <c r="F18" s="1">
+        <v>51185.933780129999</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1304100223698</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1304100223698</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1034151477392</v>
+      </c>
+      <c r="J18" s="1">
+        <v>154219734193.70001</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>0.82758620689660001</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>5929.8851430220002</v>
+      </c>
+      <c r="E19" s="1">
+        <v>48122.799173200001</v>
+      </c>
+      <c r="F19" s="1">
+        <v>48122.799173200001</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1226058577661</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1226058577661</v>
+      </c>
+      <c r="I19" s="1">
+        <v>972264452085.40002</v>
+      </c>
+      <c r="J19" s="1">
+        <v>151079876255.29999</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>0.82759310344829995</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>5214.1351734379996</v>
+      </c>
+      <c r="E20" s="1">
+        <v>42351.701688929999</v>
+      </c>
+      <c r="F20" s="1">
+        <v>42351.701688929999</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1079024246852</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1079024246852</v>
+      </c>
+      <c r="I20" s="1">
+        <v>855666227753.40002</v>
+      </c>
+      <c r="J20" s="1">
+        <v>132844208240.5</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>0.93103448275860001</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4842.4197618349999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>33924.38945147</v>
+      </c>
+      <c r="F21" s="1">
+        <v>33924.38945147</v>
+      </c>
+      <c r="G21" s="1">
+        <v>864315654814.59998</v>
+      </c>
+      <c r="H21" s="1">
+        <v>864315654814.59998</v>
+      </c>
+      <c r="I21" s="1">
+        <v>685402314267.90002</v>
+      </c>
+      <c r="J21" s="1">
+        <v>123373751893.89999</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>0.93104137931029995</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5651.3771468340001</v>
+      </c>
+      <c r="E22" s="1">
+        <v>39544.488507610004</v>
+      </c>
+      <c r="F22" s="1">
+        <v>39544.488507610004</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1007502891914</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1007502891914</v>
+      </c>
+      <c r="I22" s="1">
+        <v>798949793287.5</v>
+      </c>
+      <c r="J22" s="1">
+        <v>143984131129.5</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
         <v>1</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>4547.0611569749999</v>
-      </c>
-      <c r="E14" s="1">
-        <v>22349.511609100002</v>
-      </c>
-      <c r="F14" s="1">
-        <v>22349.511609100002</v>
-      </c>
-      <c r="G14" s="1">
-        <v>569414308512.09998</v>
-      </c>
-      <c r="H14" s="1">
-        <v>569414308512.09998</v>
-      </c>
-      <c r="I14" s="1">
-        <v>451545546650.09998</v>
-      </c>
-      <c r="J14" s="1">
-        <v>115848691897.39999</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0</v>
-      </c>
-      <c r="L14" s="1">
-        <v>0</v>
-      </c>
-      <c r="M14" s="1">
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>5050.9513737710004</v>
+      </c>
+      <c r="E23" s="1">
+        <v>28232.18459683</v>
+      </c>
+      <c r="F23" s="1">
+        <v>28232.18459683</v>
+      </c>
+      <c r="G23" s="1">
+        <v>719291327307.69995</v>
+      </c>
+      <c r="H23" s="1">
+        <v>719291327307.69995</v>
+      </c>
+      <c r="I23" s="1">
+        <v>570398022555</v>
+      </c>
+      <c r="J23" s="1">
+        <v>128686659204.39999</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1327,9 +1700,9 @@
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1340,7 +1713,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1351,7 +1724,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>200000000000</v>
       </c>

</xml_diff>

<commit_message>
Updated OpenFAST model with generator/nacelle redesign, monopile/tower redesign, and controller updates
</commit_message>
<xml_diff>
--- a/Documentation/tower_data.xlsx
+++ b/Documentation/tower_data.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egaertne\WISDEM2\wisdem\NREL15mw_ORWT\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egaertne\Projects\IEA15MW_dlc\IEA-15-240-RWT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93CE2F1-D5BE-4C92-A95D-204F6C51CC73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23803A61-5EE8-4194-829F-F12B0A7F4E6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7BFE80E2-434A-464C-9DED-2A26FA0A145D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BFE80E2-434A-464C-9DED-2A26FA0A145D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tower_Geometry" sheetId="1" r:id="rId1"/>
     <sheet name="Tower_Elastic_Properties" sheetId="4" r:id="rId2"/>
     <sheet name="Materials" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Tower_Elastic_Properties!$A$4:$A$23</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Tower_Elastic_Properties!$D$4:$D$23</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Height</t>
   </si>
@@ -130,6 +126,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,13 +164,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -488,281 +487,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED6BB49-C631-4A05-A4BA-B5BF79F8585F}">
-  <dimension ref="A2:E23"/>
+  <dimension ref="A2:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.7265625" customWidth="1"/>
-    <col min="3" max="3" width="3.26953125" customWidth="1"/>
-    <col min="4" max="5" width="10.7265625" customWidth="1"/>
+    <col min="1" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
-        <v>0</v>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>20</v>
       </c>
       <c r="B4" s="5">
-        <v>4.9226890000000002E-2</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
-        <v>15</v>
+      <c r="C4" s="5">
+        <v>4.312129E-2</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>32.5</v>
       </c>
       <c r="B5" s="5">
-        <v>4.9226890000000002E-2</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>9.9999939999999992</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
-        <v>15</v>
+        <v>9.8457177100000006</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4.312129E-2</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>32.500100000000003</v>
       </c>
       <c r="B6" s="5">
-        <v>4.5814819999999999E-2</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6">
-        <v>30</v>
-      </c>
-      <c r="E6">
-        <v>9.8932979999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
-        <v>30</v>
+        <v>9.8457177100000006</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4.0988169999999997E-2</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>45</v>
       </c>
       <c r="B7" s="5">
-        <v>4.5814819999999999E-2</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7">
-        <v>45</v>
-      </c>
-      <c r="E7">
-        <v>9.5012270000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
-        <v>30</v>
+        <v>9.4700325599999999</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4.0988169999999997E-2</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>45.000100000000003</v>
       </c>
       <c r="B8" s="5">
-        <v>4.3013370000000002E-2</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8">
-        <v>60</v>
-      </c>
-      <c r="E8">
-        <v>9.0738160000000008</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
-        <v>45</v>
+        <v>9.4700325599999999</v>
+      </c>
+      <c r="C8" s="5">
+        <v>3.9651579999999999E-2</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>57.5</v>
       </c>
       <c r="B9" s="5">
-        <v>4.3013370000000002E-2</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9">
-        <v>75</v>
-      </c>
-      <c r="E9">
-        <v>8.7337340000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="5">
-        <v>45</v>
+        <v>9.0410153900000001</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3.9651579999999999E-2</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>57.500100000000003</v>
       </c>
       <c r="B10" s="5">
-        <v>4.129422E-2</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10">
-        <v>90</v>
-      </c>
-      <c r="E10">
-        <v>8.4812589999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>60</v>
+        <v>9.0410153900000001</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3.8354939999999997E-2</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>70</v>
       </c>
       <c r="B11" s="5">
-        <v>4.129422E-2</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11">
-        <v>105</v>
-      </c>
-      <c r="E11">
-        <v>8.2546970000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="5">
-        <v>60</v>
+        <v>8.5638335399999992</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3.8354939999999997E-2</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>70.000100000000003</v>
       </c>
       <c r="B12" s="5">
-        <v>3.9396180000000003E-2</v>
-      </c>
-      <c r="D12">
+        <v>8.5638335399999992</v>
+      </c>
+      <c r="C12" s="5">
+        <v>3.697131E-2</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>82.5</v>
+      </c>
+      <c r="B13" s="5">
+        <v>8.1837546099999994</v>
+      </c>
+      <c r="C13" s="5">
+        <v>3.697131E-2</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>82.500100000000003</v>
+      </c>
+      <c r="B14" s="5">
+        <v>8.1837546099999994</v>
+      </c>
+      <c r="C14" s="5">
+        <v>3.4757639999999999E-2</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>95</v>
+      </c>
+      <c r="B15" s="5">
+        <v>8.0589466200000004</v>
+      </c>
+      <c r="C15" s="5">
+        <v>3.4757639999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>95.000100000000003</v>
+      </c>
+      <c r="B16" s="5">
+        <v>8.0589466200000004</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3.1320870000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>107.5</v>
+      </c>
+      <c r="B17" s="5">
+        <v>7.92133368</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3.1320870000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>107.5001</v>
+      </c>
+      <c r="B18" s="5">
+        <v>7.92133368</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2.7932169999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>120</v>
       </c>
-      <c r="E12">
-        <v>8.0872309999999992</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5">
-        <v>75</v>
-      </c>
-      <c r="B13" s="5">
-        <v>3.9396180000000003E-2</v>
-      </c>
-      <c r="D13">
-        <v>135</v>
-      </c>
-      <c r="E13">
-        <v>7.5125270000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="5">
-        <v>75</v>
-      </c>
-      <c r="B14" s="5">
-        <v>3.6754719999999998E-2</v>
-      </c>
-      <c r="D14">
-        <v>145</v>
-      </c>
-      <c r="E14">
-        <v>6.7175479999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
-        <v>90</v>
-      </c>
-      <c r="B15" s="5">
-        <v>3.6754719999999998E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="5">
-        <v>90</v>
-      </c>
-      <c r="B16" s="5">
-        <v>3.345327E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="5">
-        <v>105</v>
-      </c>
-      <c r="B17" s="5">
-        <v>3.345327E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="5">
-        <v>105</v>
-      </c>
-      <c r="B18" s="5">
-        <v>2.984231E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="5">
-        <v>120</v>
-      </c>
       <c r="B19" s="5">
-        <v>2.984231E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="5">
-        <v>120</v>
+        <v>7.8171297400000004</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2.7932169999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>120.0001</v>
       </c>
       <c r="B20" s="5">
-        <v>2.6228640000000001E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="5">
-        <v>135</v>
+        <v>7.8171297400000004</v>
+      </c>
+      <c r="C20" s="5">
+        <v>2.475026E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>132.5</v>
       </c>
       <c r="B21" s="5">
-        <v>2.6228640000000001E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="5">
-        <v>135</v>
+        <v>7.3356343700000002</v>
+      </c>
+      <c r="C21" s="5">
+        <v>2.475026E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>132.5001</v>
       </c>
       <c r="B22" s="5">
-        <v>3.062863E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="5">
-        <v>145</v>
+        <v>7.3356343700000002</v>
+      </c>
+      <c r="C22" s="5">
+        <v>2.993388E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>146.16800000000001</v>
       </c>
       <c r="B23" s="5">
-        <v>3.062863E-2</v>
+        <v>6.5</v>
+      </c>
+      <c r="C23" s="5">
+        <v>2.993388E-2</v>
       </c>
     </row>
   </sheetData>
@@ -774,18 +771,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A7482D-9351-4154-8734-5DF3698F8469}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -826,7 +823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -867,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -878,25 +875,25 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>12080.328734090001</v>
+        <v>10588.50121511</v>
       </c>
       <c r="E4" s="1">
-        <v>149524.7351668</v>
+        <v>131219.7127956</v>
       </c>
       <c r="F4" s="1">
-        <v>149524.7351668</v>
+        <v>131219.7127956</v>
       </c>
       <c r="G4" s="1">
-        <v>3809547392784</v>
+        <v>3343177396065</v>
       </c>
       <c r="H4" s="1">
-        <v>3809547392784</v>
+        <v>3343177396065</v>
       </c>
       <c r="I4" s="1">
-        <v>3020971082478</v>
+        <v>2651139675080</v>
       </c>
       <c r="J4" s="1">
-        <v>307779076027.90002</v>
+        <v>269770731595.10001</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -908,9 +905,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>0.10344827586209999</v>
+        <v>0.1</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -919,25 +916,25 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>12080.321450040001</v>
+        <v>10424.43190557</v>
       </c>
       <c r="E5" s="1">
-        <v>149524.46469540001</v>
+        <v>125214.0489673</v>
       </c>
       <c r="F5" s="1">
-        <v>149524.46469540001</v>
+        <v>125214.0489673</v>
       </c>
       <c r="G5" s="1">
-        <v>3809540501792</v>
+        <v>3190166852671</v>
       </c>
       <c r="H5" s="1">
-        <v>3809540501792</v>
+        <v>3190166852671</v>
       </c>
       <c r="I5" s="1">
-        <v>3020965617921</v>
+        <v>2529802314168</v>
       </c>
       <c r="J5" s="1">
-        <v>307778890446.90002</v>
+        <v>265590621797.89999</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -949,9 +946,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.10345517241380001</v>
+        <v>0.1000008</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -960,25 +957,25 @@
         <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>11246.843648689999</v>
+        <v>9910.9132900650002</v>
       </c>
       <c r="E6" s="1">
-        <v>139302.90007800001</v>
+        <v>119097.46453690001</v>
       </c>
       <c r="F6" s="1">
-        <v>139302.90007800001</v>
+        <v>119097.46453690001</v>
       </c>
       <c r="G6" s="1">
-        <v>3549118473325</v>
+        <v>3034330306674</v>
       </c>
       <c r="H6" s="1">
-        <v>3549118473325</v>
+        <v>3034330306674</v>
       </c>
       <c r="I6" s="1">
-        <v>2814450949346</v>
+        <v>2406223933192</v>
       </c>
       <c r="J6" s="1">
-        <v>286543787227.70001</v>
+        <v>252507344969.79999</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
@@ -990,9 +987,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>0.20689655172409999</v>
+        <v>0.2</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -1001,25 +998,25 @@
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>11126.299898560001</v>
+        <v>9531.1595262489991</v>
       </c>
       <c r="E7" s="1">
-        <v>134871.64993129999</v>
+        <v>105925.2063586</v>
       </c>
       <c r="F7" s="1">
-        <v>134871.64993129999</v>
+        <v>105925.2063586</v>
       </c>
       <c r="G7" s="1">
-        <v>3436220380415</v>
+        <v>2698731372192</v>
       </c>
       <c r="H7" s="1">
-        <v>3436220380415</v>
+        <v>2698731372192</v>
       </c>
       <c r="I7" s="1">
-        <v>2724922761669</v>
+        <v>2140093978149</v>
       </c>
       <c r="J7" s="1">
-        <v>283472608880.40002</v>
+        <v>242832089840.70001</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
@@ -1031,9 +1028,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.20690344827589999</v>
+        <v>0.20000080000000001</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -1042,25 +1039,25 @@
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>10448.901297980001</v>
+        <v>9221.66338025</v>
       </c>
       <c r="E8" s="1">
-        <v>126731.3834704</v>
+        <v>102514.53178249999</v>
       </c>
       <c r="F8" s="1">
-        <v>126731.3834704</v>
+        <v>102514.53178249999</v>
       </c>
       <c r="G8" s="1">
-        <v>3228825056572</v>
+        <v>2611835204650</v>
       </c>
       <c r="H8" s="1">
-        <v>3228825056572</v>
+        <v>2611835204650</v>
       </c>
       <c r="I8" s="1">
-        <v>2560458269861</v>
+        <v>2071185317288</v>
       </c>
       <c r="J8" s="1">
-        <v>266214045808.5</v>
+        <v>234946837713.39999</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
@@ -1072,9 +1069,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>0.31034482758620002</v>
+        <v>0.3</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -1083,25 +1080,25 @@
         <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>10033.03017439</v>
+        <v>8802.1414187859991</v>
       </c>
       <c r="E9" s="1">
-        <v>112193.9275275</v>
+        <v>89150.423814209993</v>
       </c>
       <c r="F9" s="1">
-        <v>112193.9275275</v>
+        <v>89150.423814209993</v>
       </c>
       <c r="G9" s="1">
-        <v>2858444013440</v>
+        <v>2271348377432</v>
       </c>
       <c r="H9" s="1">
-        <v>2858444013440</v>
+        <v>2271348377432</v>
       </c>
       <c r="I9" s="1">
-        <v>2266746102658</v>
+        <v>1801179263304</v>
       </c>
       <c r="J9" s="1">
-        <v>255618603169.20001</v>
+        <v>224258380096.5</v>
       </c>
       <c r="K9" s="1">
         <v>0</v>
@@ -1113,9 +1110,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>0.31035172413790002</v>
+        <v>0.30000080000000001</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1124,25 +1121,25 @@
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>9633.7537031859993</v>
+        <v>8515.530474055</v>
       </c>
       <c r="E10" s="1">
-        <v>107767.376841</v>
+        <v>86272.293556899996</v>
       </c>
       <c r="F10" s="1">
-        <v>107767.376841</v>
+        <v>86272.293556899996</v>
       </c>
       <c r="G10" s="1">
-        <v>2745665652001</v>
+        <v>2198020218010</v>
       </c>
       <c r="H10" s="1">
-        <v>2745665652001</v>
+        <v>2198020218010</v>
       </c>
       <c r="I10" s="1">
-        <v>2177312862037</v>
+        <v>1743030032882</v>
       </c>
       <c r="J10" s="1">
-        <v>245445954221.29999</v>
+        <v>216956190421.79999</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -1154,9 +1151,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>0.4137931034483</v>
+        <v>0.4</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -1165,25 +1162,25 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>9198.5169740649999</v>
+        <v>8064.1687229469999</v>
       </c>
       <c r="E11" s="1">
-        <v>93811.253487880007</v>
+        <v>73268.271471</v>
       </c>
       <c r="F11" s="1">
-        <v>93811.253487880007</v>
+        <v>73268.271471</v>
       </c>
       <c r="G11" s="1">
-        <v>2390095630264</v>
+        <v>1866707553401</v>
       </c>
       <c r="H11" s="1">
-        <v>2390095630264</v>
+        <v>1866707553401</v>
       </c>
       <c r="I11" s="1">
-        <v>1895345834800</v>
+        <v>1480299089847</v>
       </c>
       <c r="J11" s="1">
-        <v>234357120358.29999</v>
+        <v>205456527973.20001</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
@@ -1195,9 +1192,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>0.4138</v>
+        <v>0.40000079999999999</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -1206,25 +1203,25 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>8777.5400660449995</v>
+        <v>7774.5205287380004</v>
       </c>
       <c r="E12" s="1">
-        <v>89554.919507650004</v>
+        <v>70659.455156290001</v>
       </c>
       <c r="F12" s="1">
-        <v>89554.919507650004</v>
+        <v>70659.455156290001</v>
       </c>
       <c r="G12" s="1">
-        <v>2281654000195</v>
+        <v>1800240895702</v>
       </c>
       <c r="H12" s="1">
-        <v>2281654000195</v>
+        <v>1800240895702</v>
       </c>
       <c r="I12" s="1">
-        <v>1809351622155</v>
+        <v>1427591030291</v>
       </c>
       <c r="J12" s="1">
-        <v>223631594039.39999</v>
+        <v>198076956146.20001</v>
       </c>
       <c r="K12" s="1">
         <v>0</v>
@@ -1236,9 +1233,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>0.51724137931030001</v>
+        <v>0.5</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -1247,25 +1244,25 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>8447.1489700670008</v>
+        <v>7427.9767047470004</v>
       </c>
       <c r="E13" s="1">
-        <v>79818.23217494</v>
+        <v>61625.693428910003</v>
       </c>
       <c r="F13" s="1">
-        <v>79818.23217494</v>
+        <v>61625.693428910003</v>
       </c>
       <c r="G13" s="1">
-        <v>2033585533119</v>
+        <v>1570081361246</v>
       </c>
       <c r="H13" s="1">
-        <v>2033585533119</v>
+        <v>1570081361246</v>
       </c>
       <c r="I13" s="1">
-        <v>1612633327764</v>
+        <v>1245074519468</v>
       </c>
       <c r="J13" s="1">
-        <v>215213986498.5</v>
+        <v>189247814133.70001</v>
       </c>
       <c r="K13" s="1">
         <v>0</v>
@@ -1277,9 +1274,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>0.51724827586209998</v>
+        <v>0.50000080000000002</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -1288,25 +1285,25 @@
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>7883.1582149400001</v>
+        <v>6985.1215290700002</v>
       </c>
       <c r="E14" s="1">
-        <v>74533.789468849995</v>
+        <v>57982.934750410001</v>
       </c>
       <c r="F14" s="1">
-        <v>74533.789468849995</v>
+        <v>57982.934750410001</v>
       </c>
       <c r="G14" s="1">
-        <v>1898950050162</v>
+        <v>1477272222940</v>
       </c>
       <c r="H14" s="1">
-        <v>1898950050162</v>
+        <v>1477272222940</v>
       </c>
       <c r="I14" s="1">
-        <v>1505867389778</v>
+        <v>1171476872792</v>
       </c>
       <c r="J14" s="1">
-        <v>200844795285.10001</v>
+        <v>177964879721.5</v>
       </c>
       <c r="K14" s="1">
         <v>0</v>
@@ -1318,9 +1315,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>0.62068965517240005</v>
+        <v>0.6</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -1329,25 +1326,25 @@
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>7654.3234125070003</v>
+        <v>6878.1391628769998</v>
       </c>
       <c r="E15" s="1">
-        <v>68229.685404210002</v>
+        <v>55359.405379459997</v>
       </c>
       <c r="F15" s="1">
-        <v>68229.685404210002</v>
+        <v>55359.405379459997</v>
       </c>
       <c r="G15" s="1">
-        <v>1738335933865</v>
+        <v>1410430710305</v>
       </c>
       <c r="H15" s="1">
-        <v>1738335933865</v>
+        <v>1410430710305</v>
       </c>
       <c r="I15" s="1">
-        <v>1378500395555</v>
+        <v>1118471553272</v>
       </c>
       <c r="J15" s="1">
-        <v>195014609235.89999</v>
+        <v>175239214340.79999</v>
       </c>
       <c r="K15" s="1">
         <v>0</v>
@@ -1359,9 +1356,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>0.62069655172409999</v>
+        <v>0.6000008</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -1370,25 +1367,25 @@
         <v>0</v>
       </c>
       <c r="D16" s="1">
-        <v>6969.4939707189997</v>
+        <v>6200.6963417939996</v>
       </c>
       <c r="E16" s="1">
-        <v>62173.362132590002</v>
+        <v>49949.520398790002</v>
       </c>
       <c r="F16" s="1">
-        <v>62173.362132590002</v>
+        <v>49949.520398790002</v>
       </c>
       <c r="G16" s="1">
-        <v>1584034704015</v>
+        <v>1272599245829</v>
       </c>
       <c r="H16" s="1">
-        <v>1584034704015</v>
+        <v>1272599245829</v>
       </c>
       <c r="I16" s="1">
-        <v>1256139520284</v>
+        <v>1009171201942</v>
       </c>
       <c r="J16" s="1">
-        <v>177566725368.60001</v>
+        <v>157979524631.70001</v>
       </c>
       <c r="K16" s="1">
         <v>0</v>
@@ -1400,9 +1397,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>0.72413793103449997</v>
+        <v>0.7</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -1411,25 +1408,25 @@
         <v>0</v>
       </c>
       <c r="D17" s="1">
-        <v>6782.5909927980001</v>
+        <v>6094.4013947920002</v>
       </c>
       <c r="E17" s="1">
-        <v>57304.388171869999</v>
+        <v>47424.561948989998</v>
       </c>
       <c r="F17" s="1">
-        <v>57304.388171869999</v>
+        <v>47424.561948989998</v>
       </c>
       <c r="G17" s="1">
-        <v>1459984412022</v>
+        <v>1208269094242</v>
       </c>
       <c r="H17" s="1">
-        <v>1459984412022</v>
+        <v>1208269094242</v>
       </c>
       <c r="I17" s="1">
-        <v>1157767638734</v>
+        <v>958157391733.59998</v>
       </c>
       <c r="J17" s="1">
-        <v>172804866058.5</v>
+        <v>155271373115.70001</v>
       </c>
       <c r="K17" s="1">
         <v>0</v>
@@ -1441,9 +1438,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>0.72414482758620002</v>
+        <v>0.70000079999999998</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -1452,25 +1449,25 @@
         <v>0</v>
       </c>
       <c r="D18" s="1">
-        <v>6053.1245671030001</v>
+        <v>5437.3639118359997</v>
       </c>
       <c r="E18" s="1">
-        <v>51185.933780129999</v>
+        <v>42347.935270169997</v>
       </c>
       <c r="F18" s="1">
-        <v>51185.933780129999</v>
+        <v>42347.935270169997</v>
       </c>
       <c r="G18" s="1">
-        <v>1304100223698</v>
+        <v>1078928287138</v>
       </c>
       <c r="H18" s="1">
-        <v>1304100223698</v>
+        <v>1078928287138</v>
       </c>
       <c r="I18" s="1">
-        <v>1034151477392</v>
+        <v>855590131700.59998</v>
       </c>
       <c r="J18" s="1">
-        <v>154219734193.70001</v>
+        <v>138531564632.79999</v>
       </c>
       <c r="K18" s="1">
         <v>0</v>
@@ -1482,9 +1479,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>0.82758620689660001</v>
+        <v>0.8</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -1493,25 +1490,25 @@
         <v>0</v>
       </c>
       <c r="D19" s="1">
-        <v>5929.8851430220002</v>
+        <v>5365.5831032570004</v>
       </c>
       <c r="E19" s="1">
-        <v>48122.799173200001</v>
+        <v>40692.836443300002</v>
       </c>
       <c r="F19" s="1">
-        <v>48122.799173200001</v>
+        <v>40692.836443300002</v>
       </c>
       <c r="G19" s="1">
-        <v>1226058577661</v>
+        <v>1036760164161</v>
       </c>
       <c r="H19" s="1">
-        <v>1226058577661</v>
+        <v>1036760164161</v>
       </c>
       <c r="I19" s="1">
-        <v>972264452085.40002</v>
+        <v>822150810179.40002</v>
       </c>
       <c r="J19" s="1">
-        <v>151079876255.29999</v>
+        <v>136702754223.10001</v>
       </c>
       <c r="K19" s="1">
         <v>0</v>
@@ -1523,9 +1520,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>0.82759310344829995</v>
+        <v>0.80000079999999996</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -1534,25 +1531,25 @@
         <v>0</v>
       </c>
       <c r="D20" s="1">
-        <v>5214.1351734379996</v>
+        <v>4756.3016361760001</v>
       </c>
       <c r="E20" s="1">
-        <v>42351.701688929999</v>
+        <v>36101.393959560002</v>
       </c>
       <c r="F20" s="1">
-        <v>42351.701688929999</v>
+        <v>36101.393959560002</v>
       </c>
       <c r="G20" s="1">
-        <v>1079024246852</v>
+        <v>919780737823.19995</v>
       </c>
       <c r="H20" s="1">
-        <v>1079024246852</v>
+        <v>919780737823.19995</v>
       </c>
       <c r="I20" s="1">
-        <v>855666227753.40002</v>
+        <v>729386125093.80005</v>
       </c>
       <c r="J20" s="1">
-        <v>132844208240.5</v>
+        <v>121179659520.39999</v>
       </c>
       <c r="K20" s="1">
         <v>0</v>
@@ -1564,9 +1561,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>0.93103448275860001</v>
+        <v>0.9</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -1575,25 +1572,25 @@
         <v>0</v>
       </c>
       <c r="D21" s="1">
-        <v>4842.4197618349999</v>
+        <v>4462.4071688929998</v>
       </c>
       <c r="E21" s="1">
-        <v>33924.38945147</v>
+        <v>29814.25655627</v>
       </c>
       <c r="F21" s="1">
-        <v>33924.38945147</v>
+        <v>29814.25655627</v>
       </c>
       <c r="G21" s="1">
-        <v>864315654814.59998</v>
+        <v>759598893153.30005</v>
       </c>
       <c r="H21" s="1">
-        <v>864315654814.59998</v>
+        <v>759598893153.30005</v>
       </c>
       <c r="I21" s="1">
-        <v>685402314267.90002</v>
+        <v>602361922270.59998</v>
       </c>
       <c r="J21" s="1">
-        <v>123373751893.89999</v>
+        <v>113691902392.2</v>
       </c>
       <c r="K21" s="1">
         <v>0</v>
@@ -1605,9 +1602,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>0.93104137931029995</v>
+        <v>0.90000080000000005</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1616,25 +1613,25 @@
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>5651.3771468340001</v>
+        <v>5393.173679218</v>
       </c>
       <c r="E22" s="1">
-        <v>39544.488507610004</v>
+        <v>35982.011450040001</v>
       </c>
       <c r="F22" s="1">
-        <v>39544.488507610004</v>
+        <v>35982.011450040001</v>
       </c>
       <c r="G22" s="1">
-        <v>1007502891914</v>
+        <v>916739145223.90002</v>
       </c>
       <c r="H22" s="1">
-        <v>1007502891914</v>
+        <v>916739145223.90002</v>
       </c>
       <c r="I22" s="1">
-        <v>798949793287.5</v>
+        <v>726974142162.59998</v>
       </c>
       <c r="J22" s="1">
-        <v>143984131129.5</v>
+        <v>137405698833.60001</v>
       </c>
       <c r="K22" s="1">
         <v>0</v>
@@ -1646,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -1657,25 +1654,25 @@
         <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>5050.9513737710004</v>
+        <v>4776.2963112090001</v>
       </c>
       <c r="E23" s="1">
-        <v>28232.18459683</v>
+        <v>24993.553572320001</v>
       </c>
       <c r="F23" s="1">
-        <v>28232.18459683</v>
+        <v>24993.553572320001</v>
       </c>
       <c r="G23" s="1">
-        <v>719291327307.69995</v>
+        <v>636778434963.5</v>
       </c>
       <c r="H23" s="1">
-        <v>719291327307.69995</v>
+        <v>636778434963.5</v>
       </c>
       <c r="I23" s="1">
-        <v>570398022555</v>
+        <v>504965298926.09998</v>
       </c>
       <c r="J23" s="1">
-        <v>128686659204.39999</v>
+        <v>121689077992.60001</v>
       </c>
       <c r="K23" s="1">
         <v>0</v>
@@ -1700,9 +1697,9 @@
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1713,7 +1710,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1724,7 +1721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>200000000000</v>
       </c>

</xml_diff>